<commit_message>
all write in excel
</commit_message>
<xml_diff>
--- a/public/01.xlsx
+++ b/public/01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="100">
   <si>
     <t xml:space="preserve">受注報告　</t>
   </si>
@@ -22,7 +22,7 @@
     <t>NO.</t>
   </si>
   <si>
-    <t>22-001</t>
+    <t>22-005</t>
   </si>
   <si>
     <t>入札</t>
@@ -37,12 +37,21 @@
     <t>作成日</t>
   </si>
   <si>
+    <t>111</t>
+  </si>
+  <si>
     <t>年</t>
   </si>
   <si>
+    <t>09</t>
+  </si>
+  <si>
     <t>月</t>
   </si>
   <si>
+    <t>30</t>
+  </si>
+  <si>
     <t>日</t>
   </si>
   <si>
@@ -61,19 +70,19 @@
     <t>工事名</t>
   </si>
   <si>
-    <t>test</t>
+    <t>サイバーパンクエッジランナーズ</t>
   </si>
   <si>
     <t>担当者</t>
   </si>
   <si>
-    <t>["B20000員工","E50000新人"]</t>
+    <t xml:space="preserve">B20000員工 C30000外人 O95485章魚燒 </t>
   </si>
   <si>
     <t>契約金額</t>
   </si>
   <si>
-    <t>6000000</t>
+    <t>80,000,000</t>
   </si>
   <si>
     <t>NTD</t>
@@ -82,13 +91,16 @@
     <t>坪数</t>
   </si>
   <si>
+    <t>400</t>
+  </si>
+  <si>
     <t>P</t>
   </si>
   <si>
     <t>坪単価</t>
   </si>
   <si>
-    <t>2000000</t>
+    <t>20,777</t>
   </si>
   <si>
     <t>新店</t>
@@ -97,9 +109,15 @@
     <t>工期</t>
   </si>
   <si>
+    <t>2022.09.08~09.08</t>
+  </si>
+  <si>
     <t>開幕日</t>
   </si>
   <si>
+    <t>2022.09.10</t>
+  </si>
+  <si>
     <t>協力業者</t>
   </si>
   <si>
@@ -130,9 +148,96 @@
     <t>支払金額</t>
   </si>
   <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>30%</t>
+  </si>
+  <si>
+    <t>大道汽車</t>
+  </si>
+  <si>
+    <t>6,000,000</t>
+  </si>
+  <si>
+    <t>車窗</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>-100,000</t>
+  </si>
+  <si>
+    <t>九州</t>
+  </si>
+  <si>
+    <t>8,800,000</t>
+  </si>
+  <si>
+    <t>水泥</t>
+  </si>
+  <si>
+    <t>-550,000</t>
+  </si>
+  <si>
+    <t>福興園</t>
+  </si>
+  <si>
+    <t>1,110,000</t>
+  </si>
+  <si>
+    <t>食物</t>
+  </si>
+  <si>
+    <t>-110,000</t>
+  </si>
+  <si>
+    <t>一成</t>
+  </si>
+  <si>
+    <t>60000</t>
+  </si>
+  <si>
+    <t>三合</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>1592700</t>
+  </si>
+  <si>
+    <t>八達</t>
+  </si>
+  <si>
+    <t>470000</t>
+  </si>
+  <si>
+    <t>75000</t>
+  </si>
+  <si>
+    <t>大基報關</t>
+  </si>
+  <si>
+    <t>300000</t>
+  </si>
+  <si>
+    <t>上海煤氣</t>
+  </si>
+  <si>
+    <t>35000</t>
+  </si>
+  <si>
     <t>合計金額</t>
   </si>
   <si>
+    <t>15,150,000</t>
+  </si>
+  <si>
     <t>総原価合計</t>
   </si>
   <si>
@@ -140,6 +245,12 @@
   </si>
   <si>
     <t>粗利額</t>
+  </si>
+  <si>
+    <t>18.94%</t>
+  </si>
+  <si>
+    <t>64,850,000</t>
   </si>
   <si>
     <t>決定契約金額</t>
@@ -2411,20 +2522,26 @@
         <v>6</v>
       </c>
       <c r="AI2" s="7"/>
-      <c r="AJ2" s="8"/>
+      <c r="AJ2" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="AK2" s="8"/>
       <c r="AL2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="AM2" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AP2" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="AQ2" s="7"/>
       <c r="AR2" s="7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -2475,7 +2592,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -2484,7 +2601,7 @@
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
@@ -2493,24 +2610,24 @@
       <c r="M4" s="15"/>
       <c r="N4" s="16"/>
       <c r="O4" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
       <c r="U4" s="16"/>
       <c r="V4" s="12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>
       <c r="Z4" s="14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="AA4" s="15"/>
       <c r="AB4" s="15"/>
@@ -2518,7 +2635,7 @@
       <c r="AD4" s="15"/>
       <c r="AE4" s="16"/>
       <c r="AF4" s="17" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AG4" s="18"/>
       <c r="AH4" s="18"/>
@@ -2526,7 +2643,7 @@
       <c r="AJ4" s="18"/>
       <c r="AK4" s="18"/>
       <c r="AL4" s="19" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="AM4" s="20"/>
       <c r="AN4" s="20"/>
@@ -2537,7 +2654,7 @@
     </row>
     <row r="5" ht="17.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -2546,47 +2663,47 @@
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
       <c r="H5" s="23" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I5" s="24"/>
       <c r="J5" s="24"/>
       <c r="K5" s="24"/>
       <c r="L5" s="24"/>
       <c r="M5" s="25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N5" s="26"/>
       <c r="O5" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
-      <c r="R5" s="27">
-        <v>200</v>
+      <c r="R5" s="27" t="s">
+        <v>25</v>
       </c>
       <c r="S5" s="28"/>
       <c r="T5" s="28"/>
       <c r="U5" s="29" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="V5" s="12" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
       <c r="Y5" s="13"/>
       <c r="Z5" s="23" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AA5" s="30"/>
       <c r="AB5" s="30"/>
       <c r="AC5" s="31"/>
       <c r="AD5" s="25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="AE5" s="26"/>
       <c r="AF5" s="32" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AG5" s="33"/>
       <c r="AH5" s="33"/>
@@ -2603,11 +2720,13 @@
     </row>
     <row r="6" ht="17.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="34"/>
+      <c r="D6" s="34" t="s">
+        <v>31</v>
+      </c>
       <c r="E6" s="36"/>
       <c r="F6" s="36"/>
       <c r="G6" s="36"/>
@@ -2622,19 +2741,19 @@
       <c r="P6" s="36"/>
       <c r="Q6" s="37"/>
       <c r="R6" s="38" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="S6" s="39"/>
       <c r="T6" s="39"/>
       <c r="U6" s="39"/>
-      <c r="V6" s="40">
-        <v>44813.66666666667</v>
+      <c r="V6" s="40" t="s">
+        <v>33</v>
       </c>
       <c r="W6" s="41"/>
       <c r="X6" s="41"/>
       <c r="Y6" s="42"/>
       <c r="Z6" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="AA6" s="13"/>
       <c r="AB6" s="13"/>
@@ -2642,7 +2761,7 @@
       <c r="AD6" s="13"/>
       <c r="AE6" s="13"/>
       <c r="AF6" s="34" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="AG6" s="13"/>
       <c r="AH6" s="13"/>
@@ -2659,7 +2778,7 @@
     </row>
     <row r="7" ht="17.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B7" s="36"/>
       <c r="C7" s="36"/>
@@ -2678,7 +2797,7 @@
       <c r="P7" s="36"/>
       <c r="Q7" s="43"/>
       <c r="R7" s="12" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="S7" s="36"/>
       <c r="T7" s="36"/>
@@ -2700,7 +2819,7 @@
       <c r="AJ7" s="45"/>
       <c r="AK7" s="46"/>
       <c r="AL7" s="12" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="AM7" s="47"/>
       <c r="AN7" s="47"/>
@@ -2711,7 +2830,7 @@
     </row>
     <row r="8" ht="17.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -2720,10 +2839,10 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="48" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I8" s="36" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
@@ -2731,10 +2850,10 @@
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
       <c r="O8" s="48" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="P8" s="36" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="Q8" s="36"/>
       <c r="R8" s="36"/>
@@ -2743,7 +2862,7 @@
       <c r="U8" s="36"/>
       <c r="V8" s="49"/>
       <c r="W8" s="36" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="X8" s="13"/>
       <c r="Y8" s="13"/>
@@ -2751,11 +2870,11 @@
       <c r="AA8" s="13"/>
       <c r="AB8" s="50"/>
       <c r="AC8" s="36" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="AD8" s="36"/>
       <c r="AE8" s="51" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="AF8" s="13"/>
       <c r="AG8" s="13"/>
@@ -2764,7 +2883,7 @@
       <c r="AJ8" s="13"/>
       <c r="AK8" s="50"/>
       <c r="AL8" s="36" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="AM8" s="13"/>
       <c r="AN8" s="13"/>
@@ -2866,7 +2985,9 @@
       <c r="AR10" s="73"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
+      <c r="A11" s="74" t="s">
+        <v>14</v>
+      </c>
       <c r="B11" s="70"/>
       <c r="C11" s="70"/>
       <c r="D11" s="70"/>
@@ -2874,21 +2995,29 @@
       <c r="F11" s="70"/>
       <c r="G11" s="78"/>
       <c r="H11" s="77"/>
-      <c r="I11" s="79"/>
+      <c r="I11" s="79" t="s">
+        <v>22</v>
+      </c>
       <c r="J11" s="70"/>
       <c r="K11" s="70"/>
       <c r="L11" s="70"/>
       <c r="M11" s="70"/>
       <c r="N11" s="78"/>
-      <c r="O11" s="70"/>
-      <c r="P11" s="71"/>
+      <c r="O11" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11" s="71" t="s">
+        <v>45</v>
+      </c>
       <c r="Q11" s="72"/>
       <c r="R11" s="72"/>
       <c r="S11" s="72"/>
       <c r="T11" s="72"/>
       <c r="U11" s="73"/>
       <c r="V11" s="74"/>
-      <c r="W11" s="71"/>
+      <c r="W11" s="71" t="s">
+        <v>46</v>
+      </c>
       <c r="X11" s="72"/>
       <c r="Y11" s="72"/>
       <c r="Z11" s="72"/>
@@ -2896,14 +3025,18 @@
       <c r="AB11" s="75"/>
       <c r="AC11" s="80"/>
       <c r="AD11" s="81"/>
-      <c r="AE11" s="77"/>
+      <c r="AE11" s="77" t="s">
+        <v>47</v>
+      </c>
       <c r="AF11" s="70"/>
       <c r="AG11" s="70"/>
       <c r="AH11" s="70"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="70"/>
       <c r="AK11" s="78"/>
-      <c r="AL11" s="82"/>
+      <c r="AL11" s="82" t="s">
+        <v>48</v>
+      </c>
       <c r="AM11" s="82"/>
       <c r="AN11" s="82"/>
       <c r="AO11" s="82"/>
@@ -2926,8 +3059,12 @@
       <c r="L12" s="86"/>
       <c r="M12" s="86"/>
       <c r="N12" s="87"/>
-      <c r="O12" s="70"/>
-      <c r="P12" s="71"/>
+      <c r="O12" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="P12" s="71" t="s">
+        <v>50</v>
+      </c>
       <c r="Q12" s="72"/>
       <c r="R12" s="72"/>
       <c r="S12" s="72"/>
@@ -2942,7 +3079,9 @@
       <c r="AB12" s="75"/>
       <c r="AC12" s="76"/>
       <c r="AD12" s="76"/>
-      <c r="AE12" s="77"/>
+      <c r="AE12" s="77" t="s">
+        <v>51</v>
+      </c>
       <c r="AF12" s="72"/>
       <c r="AG12" s="72"/>
       <c r="AH12" s="72"/>
@@ -2972,15 +3111,21 @@
       <c r="L13" s="86"/>
       <c r="M13" s="86"/>
       <c r="N13" s="87"/>
-      <c r="O13" s="66"/>
-      <c r="P13" s="88"/>
+      <c r="O13" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="P13" s="88" t="s">
+        <v>45</v>
+      </c>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
       <c r="T13" s="89"/>
       <c r="U13" s="89"/>
       <c r="V13" s="74"/>
-      <c r="W13" s="71"/>
+      <c r="W13" s="71" t="s">
+        <v>52</v>
+      </c>
       <c r="X13" s="72"/>
       <c r="Y13" s="72"/>
       <c r="Z13" s="72"/>
@@ -2988,14 +3133,18 @@
       <c r="AB13" s="75"/>
       <c r="AC13" s="76"/>
       <c r="AD13" s="76"/>
-      <c r="AE13" s="77"/>
+      <c r="AE13" s="77" t="s">
+        <v>53</v>
+      </c>
       <c r="AF13" s="72"/>
       <c r="AG13" s="72"/>
       <c r="AH13" s="72"/>
       <c r="AI13" s="72"/>
       <c r="AJ13" s="72"/>
       <c r="AK13" s="75"/>
-      <c r="AL13" s="90"/>
+      <c r="AL13" s="90" t="s">
+        <v>54</v>
+      </c>
       <c r="AM13" s="72"/>
       <c r="AN13" s="72"/>
       <c r="AO13" s="72"/>
@@ -3034,7 +3183,9 @@
       <c r="AB14" s="75"/>
       <c r="AC14" s="76"/>
       <c r="AD14" s="76"/>
-      <c r="AE14" s="77"/>
+      <c r="AE14" s="77" t="s">
+        <v>55</v>
+      </c>
       <c r="AF14" s="72"/>
       <c r="AG14" s="72"/>
       <c r="AH14" s="72"/>
@@ -3072,7 +3223,9 @@
       <c r="T15" s="92"/>
       <c r="U15" s="92"/>
       <c r="V15" s="74"/>
-      <c r="W15" s="71"/>
+      <c r="W15" s="71" t="s">
+        <v>56</v>
+      </c>
       <c r="X15" s="72"/>
       <c r="Y15" s="72"/>
       <c r="Z15" s="72"/>
@@ -3080,14 +3233,18 @@
       <c r="AB15" s="75"/>
       <c r="AC15" s="76"/>
       <c r="AD15" s="76"/>
-      <c r="AE15" s="77"/>
+      <c r="AE15" s="77" t="s">
+        <v>57</v>
+      </c>
       <c r="AF15" s="72"/>
       <c r="AG15" s="72"/>
       <c r="AH15" s="72"/>
       <c r="AI15" s="72"/>
       <c r="AJ15" s="72"/>
       <c r="AK15" s="75"/>
-      <c r="AL15" s="72"/>
+      <c r="AL15" s="72" t="s">
+        <v>58</v>
+      </c>
       <c r="AM15" s="72"/>
       <c r="AN15" s="72"/>
       <c r="AO15" s="72"/>
@@ -3126,7 +3283,9 @@
       <c r="AB16" s="75"/>
       <c r="AC16" s="76"/>
       <c r="AD16" s="76"/>
-      <c r="AE16" s="77"/>
+      <c r="AE16" s="77" t="s">
+        <v>59</v>
+      </c>
       <c r="AF16" s="72"/>
       <c r="AG16" s="72"/>
       <c r="AH16" s="72"/>
@@ -3164,7 +3323,9 @@
       <c r="T17" s="72"/>
       <c r="U17" s="72"/>
       <c r="V17" s="74"/>
-      <c r="W17" s="71"/>
+      <c r="W17" s="71" t="s">
+        <v>60</v>
+      </c>
       <c r="X17" s="72"/>
       <c r="Y17" s="72"/>
       <c r="Z17" s="72"/>
@@ -3172,14 +3333,18 @@
       <c r="AB17" s="75"/>
       <c r="AC17" s="76"/>
       <c r="AD17" s="76"/>
-      <c r="AE17" s="77"/>
+      <c r="AE17" s="77" t="s">
+        <v>61</v>
+      </c>
       <c r="AF17" s="72"/>
       <c r="AG17" s="72"/>
       <c r="AH17" s="72"/>
       <c r="AI17" s="72"/>
       <c r="AJ17" s="72"/>
       <c r="AK17" s="75"/>
-      <c r="AL17" s="90"/>
+      <c r="AL17" s="90" t="s">
+        <v>49</v>
+      </c>
       <c r="AM17" s="72"/>
       <c r="AN17" s="72"/>
       <c r="AO17" s="72"/>
@@ -3218,7 +3383,9 @@
       <c r="AB18" s="75"/>
       <c r="AC18" s="76"/>
       <c r="AD18" s="76"/>
-      <c r="AE18" s="77"/>
+      <c r="AE18" s="77" t="s">
+        <v>49</v>
+      </c>
       <c r="AF18" s="72"/>
       <c r="AG18" s="72"/>
       <c r="AH18" s="72"/>
@@ -3256,7 +3423,9 @@
       <c r="T19" s="72"/>
       <c r="U19" s="72"/>
       <c r="V19" s="74"/>
-      <c r="W19" s="71"/>
+      <c r="W19" s="71" t="s">
+        <v>62</v>
+      </c>
       <c r="X19" s="72"/>
       <c r="Y19" s="72"/>
       <c r="Z19" s="72"/>
@@ -3264,14 +3433,18 @@
       <c r="AB19" s="75"/>
       <c r="AC19" s="76"/>
       <c r="AD19" s="76"/>
-      <c r="AE19" s="77"/>
+      <c r="AE19" s="77" t="s">
+        <v>63</v>
+      </c>
       <c r="AF19" s="72"/>
       <c r="AG19" s="72"/>
       <c r="AH19" s="72"/>
       <c r="AI19" s="72"/>
       <c r="AJ19" s="72"/>
       <c r="AK19" s="75"/>
-      <c r="AL19" s="72"/>
+      <c r="AL19" s="72" t="s">
+        <v>49</v>
+      </c>
       <c r="AM19" s="72"/>
       <c r="AN19" s="72"/>
       <c r="AO19" s="72"/>
@@ -3310,7 +3483,9 @@
       <c r="AB20" s="75"/>
       <c r="AC20" s="76"/>
       <c r="AD20" s="76"/>
-      <c r="AE20" s="77"/>
+      <c r="AE20" s="77" t="s">
+        <v>49</v>
+      </c>
       <c r="AF20" s="72"/>
       <c r="AG20" s="72"/>
       <c r="AH20" s="72"/>
@@ -3348,7 +3523,9 @@
       <c r="T21" s="72"/>
       <c r="U21" s="72"/>
       <c r="V21" s="74"/>
-      <c r="W21" s="71"/>
+      <c r="W21" s="71" t="s">
+        <v>52</v>
+      </c>
       <c r="X21" s="72"/>
       <c r="Y21" s="72"/>
       <c r="Z21" s="72"/>
@@ -3356,14 +3533,18 @@
       <c r="AB21" s="75"/>
       <c r="AC21" s="76"/>
       <c r="AD21" s="76"/>
-      <c r="AE21" s="77"/>
+      <c r="AE21" s="77" t="s">
+        <v>64</v>
+      </c>
       <c r="AF21" s="72"/>
       <c r="AG21" s="72"/>
       <c r="AH21" s="72"/>
       <c r="AI21" s="72"/>
       <c r="AJ21" s="72"/>
       <c r="AK21" s="75"/>
-      <c r="AL21" s="72"/>
+      <c r="AL21" s="72" t="s">
+        <v>49</v>
+      </c>
       <c r="AM21" s="72"/>
       <c r="AN21" s="72"/>
       <c r="AO21" s="72"/>
@@ -3402,7 +3583,9 @@
       <c r="AB22" s="75"/>
       <c r="AC22" s="76"/>
       <c r="AD22" s="76"/>
-      <c r="AE22" s="77"/>
+      <c r="AE22" s="77" t="s">
+        <v>49</v>
+      </c>
       <c r="AF22" s="72"/>
       <c r="AG22" s="72"/>
       <c r="AH22" s="72"/>
@@ -3440,7 +3623,9 @@
       <c r="T23" s="72"/>
       <c r="U23" s="72"/>
       <c r="V23" s="74"/>
-      <c r="W23" s="71"/>
+      <c r="W23" s="71" t="s">
+        <v>65</v>
+      </c>
       <c r="X23" s="72"/>
       <c r="Y23" s="72"/>
       <c r="Z23" s="72"/>
@@ -3448,14 +3633,18 @@
       <c r="AB23" s="75"/>
       <c r="AC23" s="76"/>
       <c r="AD23" s="76"/>
-      <c r="AE23" s="77"/>
+      <c r="AE23" s="77" t="s">
+        <v>66</v>
+      </c>
       <c r="AF23" s="72"/>
       <c r="AG23" s="72"/>
       <c r="AH23" s="72"/>
       <c r="AI23" s="72"/>
       <c r="AJ23" s="72"/>
       <c r="AK23" s="75"/>
-      <c r="AL23" s="72"/>
+      <c r="AL23" s="72" t="s">
+        <v>49</v>
+      </c>
       <c r="AM23" s="72"/>
       <c r="AN23" s="72"/>
       <c r="AO23" s="72"/>
@@ -3494,7 +3683,9 @@
       <c r="AB24" s="75"/>
       <c r="AC24" s="76"/>
       <c r="AD24" s="76"/>
-      <c r="AE24" s="77"/>
+      <c r="AE24" s="77" t="s">
+        <v>49</v>
+      </c>
       <c r="AF24" s="72"/>
       <c r="AG24" s="72"/>
       <c r="AH24" s="72"/>
@@ -3532,7 +3723,9 @@
       <c r="T25" s="72"/>
       <c r="U25" s="72"/>
       <c r="V25" s="74"/>
-      <c r="W25" s="71"/>
+      <c r="W25" s="71" t="s">
+        <v>46</v>
+      </c>
       <c r="X25" s="72"/>
       <c r="Y25" s="72"/>
       <c r="Z25" s="72"/>
@@ -3540,14 +3733,18 @@
       <c r="AB25" s="75"/>
       <c r="AC25" s="76"/>
       <c r="AD25" s="76"/>
-      <c r="AE25" s="77"/>
+      <c r="AE25" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="AF25" s="72"/>
       <c r="AG25" s="72"/>
       <c r="AH25" s="72"/>
       <c r="AI25" s="72"/>
       <c r="AJ25" s="72"/>
       <c r="AK25" s="75"/>
-      <c r="AL25" s="72"/>
+      <c r="AL25" s="72" t="s">
+        <v>49</v>
+      </c>
       <c r="AM25" s="72"/>
       <c r="AN25" s="72"/>
       <c r="AO25" s="72"/>
@@ -3586,7 +3783,9 @@
       <c r="AB26" s="75"/>
       <c r="AC26" s="76"/>
       <c r="AD26" s="76"/>
-      <c r="AE26" s="77"/>
+      <c r="AE26" s="77" t="s">
+        <v>49</v>
+      </c>
       <c r="AF26" s="72"/>
       <c r="AG26" s="72"/>
       <c r="AH26" s="72"/>
@@ -3624,7 +3823,9 @@
       <c r="T27" s="92"/>
       <c r="U27" s="92"/>
       <c r="V27" s="74"/>
-      <c r="W27" s="71"/>
+      <c r="W27" s="71" t="s">
+        <v>68</v>
+      </c>
       <c r="X27" s="72"/>
       <c r="Y27" s="72"/>
       <c r="Z27" s="72"/>
@@ -3632,14 +3833,18 @@
       <c r="AB27" s="75"/>
       <c r="AC27" s="76"/>
       <c r="AD27" s="76"/>
-      <c r="AE27" s="77"/>
+      <c r="AE27" s="77" t="s">
+        <v>69</v>
+      </c>
       <c r="AF27" s="72"/>
       <c r="AG27" s="72"/>
       <c r="AH27" s="72"/>
       <c r="AI27" s="72"/>
       <c r="AJ27" s="72"/>
       <c r="AK27" s="75"/>
-      <c r="AL27" s="90"/>
+      <c r="AL27" s="90" t="s">
+        <v>49</v>
+      </c>
       <c r="AM27" s="72"/>
       <c r="AN27" s="72"/>
       <c r="AO27" s="72"/>
@@ -3678,7 +3883,9 @@
       <c r="AB28" s="75"/>
       <c r="AC28" s="76"/>
       <c r="AD28" s="76"/>
-      <c r="AE28" s="77"/>
+      <c r="AE28" s="77" t="s">
+        <v>49</v>
+      </c>
       <c r="AF28" s="72"/>
       <c r="AG28" s="72"/>
       <c r="AH28" s="72"/>
@@ -3716,7 +3923,9 @@
       <c r="T29" s="92"/>
       <c r="U29" s="92"/>
       <c r="V29" s="74"/>
-      <c r="W29" s="71"/>
+      <c r="W29" s="71" t="s">
+        <v>70</v>
+      </c>
       <c r="X29" s="72"/>
       <c r="Y29" s="72"/>
       <c r="Z29" s="72"/>
@@ -3724,14 +3933,18 @@
       <c r="AB29" s="75"/>
       <c r="AC29" s="76"/>
       <c r="AD29" s="76"/>
-      <c r="AE29" s="77"/>
+      <c r="AE29" s="77" t="s">
+        <v>71</v>
+      </c>
       <c r="AF29" s="72"/>
       <c r="AG29" s="72"/>
       <c r="AH29" s="72"/>
       <c r="AI29" s="72"/>
       <c r="AJ29" s="72"/>
       <c r="AK29" s="75"/>
-      <c r="AL29" s="90"/>
+      <c r="AL29" s="90" t="s">
+        <v>49</v>
+      </c>
       <c r="AM29" s="72"/>
       <c r="AN29" s="72"/>
       <c r="AO29" s="72"/>
@@ -3770,7 +3983,9 @@
       <c r="AB30" s="75"/>
       <c r="AC30" s="76"/>
       <c r="AD30" s="76"/>
-      <c r="AE30" s="77"/>
+      <c r="AE30" s="77" t="s">
+        <v>49</v>
+      </c>
       <c r="AF30" s="72"/>
       <c r="AG30" s="72"/>
       <c r="AH30" s="72"/>
@@ -3879,7 +4094,7 @@
     </row>
     <row r="33" ht="18" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A33" s="109" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B33" s="110"/>
       <c r="C33" s="110"/>
@@ -3888,9 +4103,8 @@
       <c r="F33" s="110"/>
       <c r="G33" s="110"/>
       <c r="H33" s="111"/>
-      <c r="I33" s="112">
-        <f>SUM(I9:I32)</f>
-        <v>0</v>
+      <c r="I33" s="112" t="s">
+        <v>22</v>
       </c>
       <c r="J33" s="113"/>
       <c r="K33" s="113"/>
@@ -3913,7 +4127,9 @@
       <c r="AB33" s="122"/>
       <c r="AC33" s="123"/>
       <c r="AD33" s="123"/>
-      <c r="AE33" s="124"/>
+      <c r="AE33" s="124" t="s">
+        <v>73</v>
+      </c>
       <c r="AF33" s="125"/>
       <c r="AG33" s="125"/>
       <c r="AH33" s="125"/>
@@ -3951,7 +4167,7 @@
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
       <c r="V34" s="130" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="W34" s="18"/>
       <c r="X34" s="18"/>
@@ -3960,11 +4176,11 @@
       <c r="AA34" s="18"/>
       <c r="AB34" s="131"/>
       <c r="AC34" s="132" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="AD34" s="132"/>
       <c r="AE34" s="130" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="AF34" s="18"/>
       <c r="AG34" s="18"/>
@@ -3973,7 +4189,7 @@
       <c r="AJ34" s="18"/>
       <c r="AK34" s="131"/>
       <c r="AL34" s="17" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="AM34" s="18"/>
       <c r="AN34" s="18"/>
@@ -4004,23 +4220,31 @@
       <c r="S35" s="137"/>
       <c r="T35" s="137"/>
       <c r="U35" s="137"/>
-      <c r="V35" s="135"/>
+      <c r="V35" s="135" t="s">
+        <v>73</v>
+      </c>
       <c r="W35" s="134"/>
       <c r="X35" s="134"/>
       <c r="Y35" s="134"/>
       <c r="Z35" s="134"/>
       <c r="AA35" s="134"/>
       <c r="AB35" s="136"/>
-      <c r="AC35" s="138"/>
+      <c r="AC35" s="138" t="s">
+        <v>77</v>
+      </c>
       <c r="AD35" s="139"/>
-      <c r="AE35" s="135"/>
+      <c r="AE35" s="135" t="s">
+        <v>78</v>
+      </c>
       <c r="AF35" s="137"/>
       <c r="AG35" s="137"/>
       <c r="AH35" s="137"/>
       <c r="AI35" s="137"/>
       <c r="AJ35" s="137"/>
       <c r="AK35" s="140"/>
-      <c r="AL35" s="135"/>
+      <c r="AL35" s="135" t="s">
+        <v>22</v>
+      </c>
       <c r="AM35" s="137"/>
       <c r="AN35" s="137"/>
       <c r="AO35" s="137"/>
@@ -4198,7 +4422,7 @@
       <c r="AC39" s="153"/>
       <c r="AD39" s="153"/>
       <c r="AE39" s="154" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="AF39" s="155"/>
       <c r="AG39" s="155"/>
@@ -4219,7 +4443,7 @@
     </row>
     <row r="40" ht="17.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A40" s="157" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="B40" s="158"/>
       <c r="C40" s="158"/>
@@ -4242,7 +4466,7 @@
       <c r="T40" s="158"/>
       <c r="U40" s="158"/>
       <c r="V40" s="158" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="W40" s="158"/>
       <c r="X40" s="158"/>
@@ -4253,7 +4477,7 @@
       <c r="AC40" s="119"/>
       <c r="AD40" s="160"/>
       <c r="AE40" s="154" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="AF40" s="154"/>
       <c r="AG40" s="154"/>
@@ -4265,12 +4489,12 @@
       <c r="AM40" s="36"/>
       <c r="AN40" s="36"/>
       <c r="AO40" s="36" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AP40" s="36"/>
       <c r="AQ40" s="36"/>
       <c r="AR40" s="43" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.25">
@@ -4367,7 +4591,7 @@
     </row>
     <row r="43" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
@@ -4461,7 +4685,7 @@
     </row>
     <row r="45" ht="17.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -4502,7 +4726,7 @@
       <c r="AL45" s="3"/>
       <c r="AM45" s="3"/>
       <c r="AN45" s="168" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="AO45" s="3"/>
       <c r="AP45" s="3"/>
@@ -4511,66 +4735,66 @@
     </row>
     <row r="46" ht="17.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
       <c r="E46" s="51" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F46" s="13"/>
       <c r="G46" s="50"/>
       <c r="H46" s="36" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="I46" s="13"/>
       <c r="J46" s="13"/>
       <c r="K46" s="13"/>
       <c r="L46" s="13"/>
       <c r="M46" s="51" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="N46" s="13"/>
       <c r="O46" s="13"/>
       <c r="P46" s="13"/>
       <c r="Q46" s="50"/>
       <c r="R46" s="51" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="S46" s="13"/>
       <c r="T46" s="13"/>
       <c r="U46" s="13"/>
       <c r="V46" s="50"/>
       <c r="W46" s="36" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="X46" s="13"/>
       <c r="Y46" s="13"/>
       <c r="Z46" s="13"/>
       <c r="AA46" s="13"/>
       <c r="AB46" s="51" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="AC46" s="13"/>
       <c r="AD46" s="13"/>
       <c r="AE46" s="13"/>
       <c r="AF46" s="50"/>
       <c r="AG46" s="36" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="AH46" s="13"/>
       <c r="AI46" s="13"/>
       <c r="AJ46" s="13"/>
       <c r="AK46" s="13"/>
       <c r="AL46" s="51" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="AM46" s="36"/>
       <c r="AN46" s="36"/>
       <c r="AO46" s="37"/>
       <c r="AP46" s="51" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="AQ46" s="13"/>
       <c r="AR46" s="35"/>
@@ -4620,7 +4844,7 @@
       <c r="AP47" s="175"/>
       <c r="AQ47" s="176"/>
       <c r="AR47" s="177" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" ht="17.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -4668,12 +4892,12 @@
       <c r="AP48" s="184"/>
       <c r="AQ48" s="185"/>
       <c r="AR48" s="186" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" ht="17.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -4791,28 +5015,28 @@
       <c r="W51" s="189"/>
       <c r="X51" s="190"/>
       <c r="Y51" s="191" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="Z51" s="192"/>
       <c r="AA51" s="192"/>
       <c r="AB51" s="192"/>
       <c r="AC51" s="193"/>
       <c r="AD51" s="194" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="AE51" s="192"/>
       <c r="AF51" s="192"/>
       <c r="AG51" s="192"/>
       <c r="AH51" s="193"/>
       <c r="AI51" s="194" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="AJ51" s="158"/>
       <c r="AK51" s="158"/>
       <c r="AL51" s="158"/>
       <c r="AM51" s="195"/>
       <c r="AN51" s="194" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="AO51" s="192"/>
       <c r="AP51" s="192"/>

</xml_diff>